<commit_message>
descw-1252 finalize tab38 rpt
* updates template for the model as well
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_38_rpt_PF_JVsforFiscal-Quarter.xlsx
+++ b/backend/reports/xlsx/Tab_38_rpt_PF_JVsforFiscal-Quarter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C3E3FA-4629-7342-A7C1-218F5AD301AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561F916E-DE20-F74A-806D-CF673D02B971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>{#r1=d.report[i+1]}</t>
   </si>
   <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
     <t>{#date=d.date}</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>{#q=d.report[0].quarter}</t>
+  </si>
+  <si>
+    <t>{#fy=d.fiscal}</t>
   </si>
 </sst>
 </file>
@@ -217,42 +217,42 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,7 +617,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -631,97 +631,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="62" customHeight="1" thickBot="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="12" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A3" s="5" t="s">
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" thickBot="1">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>10</v>
+      <c r="E5" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1"/>
     <row r="7" spans="1:5" ht="18" customHeight="1">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="19">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="19">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19">
+      <c r="B10" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19">
-      <c r="B10" s="11" t="s">
+    <row r="11" spans="1:5" ht="19">
+      <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19">
-      <c r="B11" s="11" t="s">
+    <row r="12" spans="1:5" ht="19">
+      <c r="B12" s="10" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19">
-      <c r="B12" s="11" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>